<commit_message>
DH lifetime increase to 80 years and necessary changes in other tables
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_HeatingTechnology_Lifetime.xlsx
+++ b/projects/test_building/input/Parameter_HeatingTechnology_Lifetime.xlsx
@@ -368,7 +368,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,10 +398,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D2" s="1">
-        <v>40</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>